<commit_message>
Slide + Baocao v2
</commit_message>
<xml_diff>
--- a/Documents/Tuan3/BaoCao3_Tuan3.xlsx
+++ b/Documents/Tuan3/BaoCao3_Tuan3.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="74">
   <si>
     <t>level</t>
   </si>
@@ -117,9 +117,6 @@
     <t>Sửa khóa học</t>
   </si>
   <si>
-    <t>Xóa khóa học</t>
-  </si>
-  <si>
     <t>Quản lý bài tập</t>
   </si>
   <si>
@@ -141,9 +138,6 @@
     <t>Sửa tài khoản</t>
   </si>
   <si>
-    <t>Xóa tài khoản</t>
-  </si>
-  <si>
     <t xml:space="preserve">Quản lý nhóm </t>
   </si>
   <si>
@@ -220,13 +214,52 @@
   </si>
   <si>
     <t>2.8.3</t>
+  </si>
+  <si>
+    <t>1.11.4</t>
+  </si>
+  <si>
+    <t>Tim kiếm nhóm</t>
+  </si>
+  <si>
+    <t>Xoá khoá học</t>
+  </si>
+  <si>
+    <t>2.4.4</t>
+  </si>
+  <si>
+    <t>Tìm kiếm khoá học</t>
+  </si>
+  <si>
+    <t>2.5.4</t>
+  </si>
+  <si>
+    <t>Tìm kiếm bài tập</t>
+  </si>
+  <si>
+    <t>Xoá tài khoản</t>
+  </si>
+  <si>
+    <t>2.7.4</t>
+  </si>
+  <si>
+    <t>Tìm kiếm tài khoản</t>
+  </si>
+  <si>
+    <t>Xoá nhóm</t>
+  </si>
+  <si>
+    <t>2.8.4</t>
+  </si>
+  <si>
+    <t>Tìm kiếm nhóm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,8 +280,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -270,12 +311,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -325,25 +360,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,10 +708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -698,172 +743,180 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="17">
+        <v>2</v>
+      </c>
+      <c r="B3" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="6">
+      <c r="A4" s="17">
+        <v>2</v>
+      </c>
+      <c r="B4" s="18">
         <v>1.2</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
-        <v>2</v>
-      </c>
-      <c r="B5" s="6">
+      <c r="A5" s="17">
+        <v>2</v>
+      </c>
+      <c r="B5" s="18">
         <v>1.4</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="17" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
-        <v>2</v>
-      </c>
-      <c r="B6" s="6">
+      <c r="A6" s="17">
+        <v>2</v>
+      </c>
+      <c r="B6" s="18">
         <v>1.5</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="17" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
-        <v>2</v>
-      </c>
-      <c r="B7" s="6">
+      <c r="A7" s="17">
+        <v>2</v>
+      </c>
+      <c r="B7" s="18">
         <v>1.6</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="17" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
-        <v>2</v>
-      </c>
-      <c r="B8" s="6">
+      <c r="A8" s="17">
+        <v>2</v>
+      </c>
+      <c r="B8" s="18">
         <v>1.7</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="17" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
-        <v>2</v>
-      </c>
-      <c r="B9" s="6">
+      <c r="A9" s="17">
+        <v>2</v>
+      </c>
+      <c r="B9" s="18">
         <v>1.8</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
-        <v>2</v>
-      </c>
-      <c r="B10" s="6">
+      <c r="A10" s="17">
+        <v>2</v>
+      </c>
+      <c r="B10" s="18">
         <v>1.9</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="17" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
-        <v>2</v>
-      </c>
-      <c r="B11" s="8" t="s">
+      <c r="A11" s="21">
+        <v>2</v>
+      </c>
+      <c r="B11" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="21" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="7">
-        <v>3</v>
-      </c>
-      <c r="B12" s="8" t="s">
+      <c r="A12" s="4">
+        <v>3</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="9">
-        <v>2</v>
-      </c>
-      <c r="B13" s="10" t="s">
+      <c r="A13" s="26">
+        <v>2</v>
+      </c>
+      <c r="B13" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="6">
+        <v>3</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
+        <v>3</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
+        <v>3</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="9">
-        <v>3</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="9">
-        <v>3</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="9">
-        <v>3</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
-        <v>2</v>
-      </c>
-      <c r="B17" s="6" t="s">
+      <c r="A17" s="6">
+        <v>3</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="17">
+        <v>2</v>
+      </c>
+      <c r="B18" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C18" s="17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
@@ -939,6 +992,9 @@
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B44" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -949,10 +1005,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -976,7 +1032,7 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -984,226 +1040,271 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="17">
+        <v>2</v>
+      </c>
+      <c r="B3" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="17">
+        <v>2</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="17">
+        <v>2</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="15">
+        <v>2</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
-        <v>2</v>
-      </c>
-      <c r="B5" s="6" t="s">
+      <c r="C6" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="9">
+        <v>3</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="12">
-        <v>2</v>
-      </c>
-      <c r="B6" s="13" t="s">
+      <c r="C7" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="9">
+        <v>3</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="12">
-        <v>3</v>
-      </c>
-      <c r="B7" s="13" t="s">
+      <c r="C8" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="12">
-        <v>3</v>
-      </c>
-      <c r="B8" s="13" t="s">
+      <c r="C9" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="9">
+        <v>3</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="19">
+        <v>2</v>
+      </c>
+      <c r="B11" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="12">
-        <v>3</v>
-      </c>
-      <c r="B9" s="13" t="s">
+      <c r="C11" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="13">
+        <v>3</v>
+      </c>
+      <c r="B12" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="14">
-        <v>2</v>
-      </c>
-      <c r="B10" s="15" t="s">
+      <c r="C12" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="13">
+        <v>3</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="14">
-        <v>3</v>
-      </c>
-      <c r="B11" s="15" t="s">
+      <c r="C13" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="13">
+        <v>3</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="14">
-        <v>3</v>
-      </c>
-      <c r="B12" s="15" t="s">
+      <c r="C14" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="13">
+        <v>3</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="17">
+        <v>2</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="14">
-        <v>3</v>
-      </c>
-      <c r="B13" s="15" t="s">
+      <c r="C16" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="21">
+        <v>2</v>
+      </c>
+      <c r="B17" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C17" s="21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
-        <v>2</v>
-      </c>
-      <c r="B14" s="6" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>3</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
-        <v>2</v>
-      </c>
-      <c r="B15" s="6" t="s">
+      <c r="C18" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <v>3</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="7">
-        <v>3</v>
-      </c>
-      <c r="B16" s="8" t="s">
+      <c r="C19" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>3</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="7">
-        <v>3</v>
-      </c>
-      <c r="B17" s="8" t="s">
+      <c r="C20" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>3</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="23">
+        <v>2</v>
+      </c>
+      <c r="B22" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C22" s="23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="7">
-        <v>3</v>
-      </c>
-      <c r="B18" s="8" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="11">
+        <v>3</v>
+      </c>
+      <c r="B23" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C23" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="16">
-        <v>2</v>
-      </c>
-      <c r="B19" s="17" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="11">
+        <v>3</v>
+      </c>
+      <c r="B24" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C24" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="16">
-        <v>3</v>
-      </c>
-      <c r="B20" s="17" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="11">
+        <v>3</v>
+      </c>
+      <c r="B25" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="16">
-        <v>3</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="16">
-        <v>3</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>40</v>
+      <c r="C25" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="11">
+        <v>3</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>